<commit_message>
added approx dates for Judges; updated book notes; updated KMZ parse script
</commit_message>
<xml_diff>
--- a/metadata/data_sources.xlsx
+++ b/metadata/data_sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIKE.MK-DESKTOP\Documents\Jobs\Data_Analytics\Patterns within the Bible\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIKE.MK-DESKTOP\Documents\Career\Data_Analytics\Projects\patterns_within_the_bible\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07303C2F-2E54-4CB0-8686-EA50EC7432E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611AAA49-2512-48D7-8A78-27D10E132EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3312" yWindow="2784" windowWidth="30960" windowHeight="12312" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20688" yWindow="252" windowWidth="20340" windowHeight="16452" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>https://www.openbible.info/geo/</t>
   </si>
@@ -71,9 +71,6 @@
     <t>https://www.christthetruth.net/2013/07/15/strongs-goes-excel/</t>
   </si>
   <si>
-    <t>wlc = "Westminster Leningrad Codex" (oldest known complete Hebrew manuscript)</t>
-  </si>
-  <si>
     <t>https://www.wilfredgraves.org/wp-content/uploads/2019/07/List-of-Miracles-Old-Testament.pdf</t>
   </si>
   <si>
@@ -117,6 +114,12 @@
   </si>
   <si>
     <t>bible scripture</t>
+  </si>
+  <si>
+    <t>Claude 4.1 for locations_no_geo.csv</t>
+  </si>
+  <si>
+    <t>wlc = "Westminster Leningrad Codex" (oldest known complete Hebrew manuscript); ESV and NRSV cannot be downloaded locally per copyright</t>
   </si>
 </sst>
 </file>
@@ -451,7 +454,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,7 +472,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -486,10 +489,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -505,10 +511,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -527,46 +533,46 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
         <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
multiple updates; added tableau dashboard prototypes
</commit_message>
<xml_diff>
--- a/metadata/data_sources.xlsx
+++ b/metadata/data_sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIKE.MK-DESKTOP\Documents\Career\Data_Analytics\Projects\patterns_within_the_bible\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611AAA49-2512-48D7-8A78-27D10E132EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADB8904-9AD3-481E-A569-EE04D5AAE715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20688" yWindow="252" windowWidth="20340" windowHeight="16452" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7584" yWindow="2760" windowWidth="32748" windowHeight="11568" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>https://www.openbible.info/geo/</t>
   </si>
@@ -120,6 +120,18 @@
   </si>
   <si>
     <t>wlc = "Westminster Leningrad Codex" (oldest known complete Hebrew manuscript); ESV and NRSV cannot be downloaded locally per copyright</t>
+  </si>
+  <si>
+    <t>rouses_metav_dataset</t>
+  </si>
+  <si>
+    <t>https://public.tableau.com/app/profile/robertrouse/viz/MetaV-app/Passages</t>
+  </si>
+  <si>
+    <t>#NEED ERD# well-built dataset of the ?KJV? Bible translation</t>
+  </si>
+  <si>
+    <t>https://github.com/robertrouse/theographic-bible-metadata</t>
   </si>
 </sst>
 </file>
@@ -451,16 +463,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.77734375" customWidth="1"/>
+    <col min="2" max="2" width="52.21875" customWidth="1"/>
     <col min="3" max="3" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -573,6 +585,20 @@
       </c>
       <c r="D9" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>